<commit_message>
refactored code, improved speed
</commit_message>
<xml_diff>
--- a/data/00_data_forModel_all.xlsx
+++ b/data/00_data_forModel_all.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tpytsui\Documents\Surfdrive\Documents\_PhD\_github\bimzec\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDB2A0B-36FA-4F4D-A4D5-6D9350462517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05C059A-F27D-4D39-854C-4465F798C247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="821" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="821" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data overview" sheetId="1" r:id="rId1"/>
@@ -426,7 +426,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -522,7 +522,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -964,7 +964,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1110,8 +1110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96C88D6-EBE3-4BD6-9917-8098B440CAD4}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1346,9 +1346,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3070A317-EA4A-4349-8291-694C61C1EC72}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
changed model.ipynb to run on binder
</commit_message>
<xml_diff>
--- a/data/00_data_forModel_all.xlsx
+++ b/data/00_data_forModel_all.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tpytsui\Documents\Surfdrive\Documents\_PhD\_github\bimzec\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05C059A-F27D-4D39-854C-4465F798C247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FCB9AB-5446-4942-9D5B-9237B725142F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="821" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="821" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data overview" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="129">
   <si>
     <t>Data overview</t>
   </si>
@@ -419,6 +419,21 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>hub_usage</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>start_year</t>
+  </si>
+  <si>
+    <t>end_year</t>
   </si>
 </sst>
 </file>
@@ -1344,11 +1359,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3070A317-EA4A-4349-8291-694C61C1EC72}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
+      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1357,10 +1372,11 @@
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="19.5546875" customWidth="1"/>
     <col min="5" max="7" width="20.44140625" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19.44140625" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -1385,8 +1401,11 @@
       <c r="H1" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1413,8 +1432,11 @@
       <c r="H2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1441,8 +1463,11 @@
       <c r="H3" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -1469,8 +1494,11 @@
       <c r="H4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -1497,8 +1525,11 @@
       <c r="H5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -1525,8 +1556,11 @@
       <c r="H6" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>60</v>
       </c>
@@ -1553,8 +1587,11 @@
       <c r="H7" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -1581,8 +1618,11 @@
       <c r="H8" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -1609,8 +1649,11 @@
       <c r="H9" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -1637,8 +1680,11 @@
       <c r="H10" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -1665,8 +1711,11 @@
       <c r="H11" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -1693,8 +1742,11 @@
       <c r="H12" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -1721,8 +1773,11 @@
       <c r="H13" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -1749,8 +1804,11 @@
       <c r="H14" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>49</v>
       </c>
@@ -1777,8 +1835,11 @@
       <c r="H15" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -1787,6 +1848,9 @@
       </c>
       <c r="H16" t="s">
         <v>120</v>
+      </c>
+      <c r="I16" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
@@ -1846,9 +1910,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A5D0406-5DCE-4EA0-A6FA-60BD40F7B812}">
   <dimension ref="A1:G173"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8086,10 +8150,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0587A319-C95B-4506-8508-A6F63244A99F}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8097,9 +8161,11 @@
     <col min="1" max="1" width="20.21875" customWidth="1"/>
     <col min="2" max="2" width="13.44140625" customWidth="1"/>
     <col min="3" max="3" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -8112,8 +8178,14 @@
       <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -8127,7 +8199,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -8141,7 +8213,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -8155,7 +8227,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -8169,7 +8241,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -8183,7 +8255,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -8197,7 +8269,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -8211,7 +8283,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -8225,7 +8297,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -8239,7 +8311,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -8253,7 +8325,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -8267,7 +8339,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -8281,7 +8353,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -8295,7 +8367,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -8309,7 +8381,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>

</xml_diff>